<commit_message>
UPDATED SPREADSHEET FOR HEAVEN COMING DOWN
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="69">
   <si>
     <t>SONG</t>
   </si>
@@ -192,13 +192,52 @@
   </si>
   <si>
     <t>All Killer No Filler</t>
+  </si>
+  <si>
+    <t>NIGHT MAGIC</t>
+  </si>
+  <si>
+    <t>91 SHOT KALEIDOSCOPE</t>
+  </si>
+  <si>
+    <t>HEAVEN'S GATE</t>
+  </si>
+  <si>
+    <t>OVER THE RAINBOW</t>
+  </si>
+  <si>
+    <t>EMPEROR'S TATTOO</t>
+  </si>
+  <si>
+    <t>MULTICOLOR PEONIES</t>
+  </si>
+  <si>
+    <t>SUNRISE FOUNTAIN</t>
+  </si>
+  <si>
+    <t>WHIRLWINDS</t>
+  </si>
+  <si>
+    <t>SILVER MONSTER</t>
+  </si>
+  <si>
+    <t>MELTDOWN</t>
+  </si>
+  <si>
+    <t>*** DENOTES PRICE FROM PHATBOY</t>
+  </si>
+  <si>
+    <t>*** DENOTES PRICE FROM FIREWORKS CENTRAL</t>
+  </si>
+  <si>
+    <t>***DENOTES UNKNOWN PRICE\AVAILABILITY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,8 +280,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,8 +331,23 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -294,14 +370,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -309,15 +403,28 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="5"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="6"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="7">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="6" builtinId="23"/>
+    <cellStyle name="Good" xfId="4" builtinId="26"/>
+    <cellStyle name="Input" xfId="5" builtinId="20"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFC7CE"/>
+      <color rgb="FFFF9999"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -592,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,267 +765,277 @@
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="H4" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <f>C5*D5</f>
+        <v>96</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4">
+        <v>27</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E16" si="0">C6*D6</f>
+        <v>270</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4">
+        <v>43</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" s="8">
         <v>0</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" s="4">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12">
         <v>1</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>32</v>
-      </c>
-      <c r="E11">
-        <f>C11*D11</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="D12" s="7">
         <v>7</v>
       </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>19</v>
-      </c>
       <c r="E12">
-        <f t="shared" ref="E12:E25" si="0">C12*D12</f>
-        <v>38</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
+      <c r="A13" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13">
         <v>8</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>33</v>
+      <c r="D13" s="4">
+        <v>65</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14">
-        <v>41</v>
+        <v>4</v>
+      </c>
+      <c r="D14" s="7">
+        <v>35</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>5</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="D15" s="5">
-        <v>65</v>
+      <c r="D15" s="10">
+        <v>55</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
       <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16">
-        <v>30</v>
+        <v>1</v>
+      </c>
+      <c r="D16" s="9">
+        <v>52</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17" s="5">
-        <v>8</v>
-      </c>
+      <c r="D17" s="1"/>
       <c r="E17">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18">
-        <v>34</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>68</v>
+        <f>SUM(E5:E16)</f>
+        <v>1466</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19">
+      <c r="A19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="2">
-        <v>30</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>30</v>
+      <c r="C19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20">
+        <v>51</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D20">
-        <v>29</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21">
-        <v>19</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22">
+      <c r="C22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D22">
-        <v>47</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>141</v>
+      <c r="E22" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -926,17 +1043,17 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
       <c r="D23">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
-        <v>58</v>
+        <f>C23*D23</f>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -944,17 +1061,17 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
         <v>19</v>
       </c>
-      <c r="C24">
-        <v>3</v>
-      </c>
-      <c r="D24">
-        <v>13</v>
-      </c>
       <c r="E24">
-        <f t="shared" si="0"/>
-        <v>39</v>
+        <f t="shared" ref="E24:E37" si="1">C24*D24</f>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -962,283 +1079,283 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="D25" s="5">
-        <v>48</v>
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>33</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
-        <v>96</v>
+        <f t="shared" si="1"/>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D26" s="1"/>
-      <c r="E26" s="6">
-        <f>SUM(E11:E25)</f>
-        <v>898</v>
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>41</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27">
         <v>1</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>4</v>
+      <c r="D27" s="5">
+        <v>65</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>30</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D29" s="1"/>
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" s="5">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>4</v>
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>34</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C31">
-        <v>3</v>
-      </c>
-      <c r="D31">
-        <v>33.5</v>
+        <v>1</v>
+      </c>
+      <c r="D31" s="2">
+        <v>30</v>
       </c>
       <c r="E31">
-        <f>C31*D31</f>
-        <v>100.5</v>
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D32">
-        <v>29.95</v>
+        <v>29</v>
       </c>
       <c r="E32">
-        <f t="shared" ref="E32:E61" si="1">C32*D32</f>
-        <v>119.8</v>
+        <f t="shared" si="1"/>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D33">
-        <v>28.75</v>
+        <v>19</v>
       </c>
       <c r="E33">
         <f t="shared" si="1"/>
-        <v>28.75</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C34">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D34">
-        <v>3.6</v>
+        <v>47</v>
       </c>
       <c r="E34">
         <f t="shared" si="1"/>
-        <v>57.6</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D35">
-        <v>28.1</v>
+        <v>29</v>
       </c>
       <c r="E35">
         <f t="shared" si="1"/>
-        <v>28.1</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D36">
-        <v>32.4</v>
+        <v>13</v>
       </c>
       <c r="E36">
         <f t="shared" si="1"/>
-        <v>64.8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C37">
-        <v>3</v>
-      </c>
-      <c r="D37">
-        <v>20.100000000000001</v>
+        <v>2</v>
+      </c>
+      <c r="D37" s="5">
+        <v>48</v>
       </c>
       <c r="E37">
         <f t="shared" si="1"/>
-        <v>60.300000000000004</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38" t="s">
-        <v>28</v>
-      </c>
-      <c r="C38">
-        <v>2</v>
-      </c>
-      <c r="D38">
-        <v>34.950000000000003</v>
-      </c>
-      <c r="E38">
-        <f t="shared" si="1"/>
-        <v>69.900000000000006</v>
+      <c r="D38" s="1"/>
+      <c r="E38" s="6">
+        <f>SUM(E23:E37)</f>
+        <v>898</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>22</v>
-      </c>
-      <c r="B39" t="s">
-        <v>29</v>
-      </c>
-      <c r="C39">
+      <c r="A39" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D39">
-        <v>36.950000000000003</v>
-      </c>
-      <c r="E39">
-        <f t="shared" si="1"/>
-        <v>36.950000000000003</v>
+      <c r="C39" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>22</v>
-      </c>
-      <c r="B40" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40">
-        <v>2</v>
-      </c>
-      <c r="D40">
-        <v>12.75</v>
-      </c>
-      <c r="E40">
-        <f t="shared" si="1"/>
-        <v>25.5</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>22</v>
-      </c>
-      <c r="B41" t="s">
-        <v>30</v>
-      </c>
-      <c r="C41">
-        <v>2</v>
-      </c>
-      <c r="D41">
-        <v>21.25</v>
-      </c>
-      <c r="E41">
-        <f t="shared" si="1"/>
-        <v>42.5</v>
-      </c>
+      <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>22</v>
-      </c>
-      <c r="B42" t="s">
-        <v>31</v>
-      </c>
-      <c r="C42">
+      <c r="A42" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D42">
-        <v>34.200000000000003</v>
-      </c>
-      <c r="E42">
-        <f t="shared" si="1"/>
-        <v>34.200000000000003</v>
+      <c r="C42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1246,17 +1363,17 @@
         <v>22</v>
       </c>
       <c r="B43" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C43">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D43">
-        <v>8.9499999999999993</v>
+        <v>33.5</v>
       </c>
       <c r="E43">
-        <f t="shared" si="1"/>
-        <v>53.699999999999996</v>
+        <f>C43*D43</f>
+        <v>100.5</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1264,17 +1381,17 @@
         <v>22</v>
       </c>
       <c r="B44" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C44">
-        <v>2</v>
-      </c>
-      <c r="D44" s="4">
-        <v>27.75</v>
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>29.95</v>
       </c>
       <c r="E44">
-        <f t="shared" si="1"/>
-        <v>55.5</v>
+        <f t="shared" ref="E44:E73" si="2">C44*D44</f>
+        <v>119.8</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1282,17 +1399,17 @@
         <v>22</v>
       </c>
       <c r="B45" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C45">
-        <v>5</v>
-      </c>
-      <c r="D45" s="4">
-        <v>10.5</v>
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>28.75</v>
       </c>
       <c r="E45">
-        <f t="shared" si="1"/>
-        <v>52.5</v>
+        <f t="shared" si="2"/>
+        <v>28.75</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1300,17 +1417,17 @@
         <v>22</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C46">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D46">
-        <v>35.950000000000003</v>
+        <v>3.6</v>
       </c>
       <c r="E46">
-        <f t="shared" si="1"/>
-        <v>71.900000000000006</v>
+        <f t="shared" si="2"/>
+        <v>57.6</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1318,17 +1435,17 @@
         <v>22</v>
       </c>
       <c r="B47" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D47">
-        <v>29.75</v>
+        <v>28.1</v>
       </c>
       <c r="E47">
-        <f t="shared" si="1"/>
-        <v>59.5</v>
+        <f t="shared" si="2"/>
+        <v>28.1</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1336,17 +1453,17 @@
         <v>22</v>
       </c>
       <c r="B48" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C48">
         <v>2</v>
       </c>
       <c r="D48">
-        <v>24.75</v>
+        <v>32.4</v>
       </c>
       <c r="E48">
-        <f t="shared" si="1"/>
-        <v>49.5</v>
+        <f t="shared" si="2"/>
+        <v>64.8</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1354,17 +1471,17 @@
         <v>22</v>
       </c>
       <c r="B49" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D49">
-        <v>28.95</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="E49">
-        <f t="shared" si="1"/>
-        <v>57.9</v>
+        <f t="shared" si="2"/>
+        <v>60.300000000000004</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1372,17 +1489,17 @@
         <v>22</v>
       </c>
       <c r="B50" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D50">
-        <v>19.95</v>
+        <v>34.950000000000003</v>
       </c>
       <c r="E50">
-        <f t="shared" si="1"/>
-        <v>19.95</v>
+        <f t="shared" si="2"/>
+        <v>69.900000000000006</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1390,17 +1507,17 @@
         <v>22</v>
       </c>
       <c r="B51" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D51">
-        <v>26.95</v>
+        <v>36.950000000000003</v>
       </c>
       <c r="E51">
-        <f>C51*D51</f>
-        <v>53.9</v>
+        <f t="shared" si="2"/>
+        <v>36.950000000000003</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1408,17 +1525,17 @@
         <v>22</v>
       </c>
       <c r="B52" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C52">
         <v>2</v>
       </c>
       <c r="D52">
-        <v>23.25</v>
+        <v>12.75</v>
       </c>
       <c r="E52">
-        <f t="shared" si="1"/>
-        <v>46.5</v>
+        <f t="shared" si="2"/>
+        <v>25.5</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1426,17 +1543,17 @@
         <v>22</v>
       </c>
       <c r="B53" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C53">
         <v>2</v>
       </c>
       <c r="D53">
-        <v>33.9</v>
+        <v>21.25</v>
       </c>
       <c r="E53">
-        <f t="shared" si="1"/>
-        <v>67.8</v>
+        <f t="shared" si="2"/>
+        <v>42.5</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1444,17 +1561,17 @@
         <v>22</v>
       </c>
       <c r="B54" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C54">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D54">
         <v>34.200000000000003</v>
       </c>
       <c r="E54">
-        <f t="shared" si="1"/>
-        <v>102.60000000000001</v>
+        <f t="shared" si="2"/>
+        <v>34.200000000000003</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1462,17 +1579,17 @@
         <v>22</v>
       </c>
       <c r="B55" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D55">
-        <v>50.85</v>
+        <v>8.9499999999999993</v>
       </c>
       <c r="E55">
-        <f t="shared" si="1"/>
-        <v>50.85</v>
+        <f t="shared" si="2"/>
+        <v>53.699999999999996</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1480,17 +1597,17 @@
         <v>22</v>
       </c>
       <c r="B56" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C56">
-        <v>4</v>
-      </c>
-      <c r="D56">
-        <v>41.1</v>
+        <v>2</v>
+      </c>
+      <c r="D56" s="4">
+        <v>27.75</v>
       </c>
       <c r="E56">
-        <f t="shared" si="1"/>
-        <v>164.4</v>
+        <f t="shared" si="2"/>
+        <v>55.5</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1498,17 +1615,17 @@
         <v>22</v>
       </c>
       <c r="B57" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C57">
-        <v>2</v>
-      </c>
-      <c r="D57">
-        <v>41.1</v>
+        <v>5</v>
+      </c>
+      <c r="D57" s="4">
+        <v>10.5</v>
       </c>
       <c r="E57">
-        <f t="shared" si="1"/>
-        <v>82.2</v>
+        <f t="shared" si="2"/>
+        <v>52.5</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1516,17 +1633,17 @@
         <v>22</v>
       </c>
       <c r="B58" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C58">
         <v>2</v>
       </c>
       <c r="D58">
-        <v>22.75</v>
+        <v>35.950000000000003</v>
       </c>
       <c r="E58">
-        <f t="shared" si="1"/>
-        <v>45.5</v>
+        <f t="shared" si="2"/>
+        <v>71.900000000000006</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1534,17 +1651,17 @@
         <v>22</v>
       </c>
       <c r="B59" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C59">
         <v>2</v>
       </c>
       <c r="D59">
-        <v>29</v>
+        <v>29.75</v>
       </c>
       <c r="E59">
-        <f t="shared" si="1"/>
-        <v>58</v>
+        <f t="shared" si="2"/>
+        <v>59.5</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1552,17 +1669,17 @@
         <v>22</v>
       </c>
       <c r="B60" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C60">
-        <v>4</v>
-      </c>
-      <c r="D60" s="4">
-        <v>10.5</v>
+        <v>2</v>
+      </c>
+      <c r="D60">
+        <v>24.75</v>
       </c>
       <c r="E60">
-        <f t="shared" si="1"/>
-        <v>42</v>
+        <f t="shared" si="2"/>
+        <v>49.5</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1570,22 +1687,238 @@
         <v>22</v>
       </c>
       <c r="B61" t="s">
+        <v>38</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+      <c r="D61">
+        <v>28.95</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>57.9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62" t="s">
+        <v>39</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>19.95</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>19.95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>22</v>
+      </c>
+      <c r="B63" t="s">
+        <v>40</v>
+      </c>
+      <c r="C63">
+        <v>2</v>
+      </c>
+      <c r="D63">
+        <v>26.95</v>
+      </c>
+      <c r="E63">
+        <f>C63*D63</f>
+        <v>53.9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>22</v>
+      </c>
+      <c r="B64" t="s">
+        <v>41</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
+      </c>
+      <c r="D64">
+        <v>23.25</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="2"/>
+        <v>46.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>22</v>
+      </c>
+      <c r="B65" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
+      </c>
+      <c r="D65">
+        <v>33.9</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="2"/>
+        <v>67.8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>22</v>
+      </c>
+      <c r="B66" t="s">
+        <v>42</v>
+      </c>
+      <c r="C66">
+        <v>3</v>
+      </c>
+      <c r="D66">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="2"/>
+        <v>102.60000000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>22</v>
+      </c>
+      <c r="B67" t="s">
+        <v>43</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>50.85</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="2"/>
+        <v>50.85</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>22</v>
+      </c>
+      <c r="B68" t="s">
+        <v>44</v>
+      </c>
+      <c r="C68">
+        <v>4</v>
+      </c>
+      <c r="D68">
+        <v>41.1</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="2"/>
+        <v>164.4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>22</v>
+      </c>
+      <c r="B69" t="s">
+        <v>45</v>
+      </c>
+      <c r="C69">
+        <v>2</v>
+      </c>
+      <c r="D69">
+        <v>41.1</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="2"/>
+        <v>82.2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>22</v>
+      </c>
+      <c r="B70" t="s">
+        <v>46</v>
+      </c>
+      <c r="C70">
+        <v>2</v>
+      </c>
+      <c r="D70">
+        <v>22.75</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="2"/>
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>22</v>
+      </c>
+      <c r="B71" t="s">
+        <v>47</v>
+      </c>
+      <c r="C71">
+        <v>2</v>
+      </c>
+      <c r="D71">
+        <v>29</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>22</v>
+      </c>
+      <c r="B72" t="s">
+        <v>48</v>
+      </c>
+      <c r="C72">
+        <v>4</v>
+      </c>
+      <c r="D72" s="4">
+        <v>10.5</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>22</v>
+      </c>
+      <c r="B73" t="s">
         <v>49</v>
       </c>
-      <c r="C61">
-        <v>2</v>
-      </c>
-      <c r="D61" s="4">
+      <c r="C73">
+        <v>2</v>
+      </c>
+      <c r="D73" s="4">
         <v>4.5</v>
       </c>
-      <c r="E61">
-        <f t="shared" si="1"/>
+      <c r="E73">
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E62" s="6">
-        <f>SUM(E31:E61)</f>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E74" s="6">
+        <f>SUM(E43:E73)</f>
         <v>1812.1000000000004</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PULLED NIGHT MAGIC FROM HEAVEN
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -194,9 +194,6 @@
     <t>All Killer No Filler</t>
   </si>
   <si>
-    <t>NIGHT MAGIC</t>
-  </si>
-  <si>
     <t>91 SHOT KALEIDOSCOPE</t>
   </si>
   <si>
@@ -231,6 +228,9 @@
   </si>
   <si>
     <t>***DENOTES UNKNOWN PRICE\AVAILABILITY</t>
+  </si>
+  <si>
+    <t>CDC-9393</t>
   </si>
 </sst>
 </file>
@@ -303,7 +303,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -344,6 +344,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -395,7 +401,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -407,6 +413,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="5"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="6"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -702,7 +709,7 @@
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,7 +773,7 @@
         <v>4</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -774,20 +781,20 @@
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5" s="5">
-        <v>16</v>
+        <v>2</v>
+      </c>
+      <c r="D5" s="11">
+        <v>35</v>
       </c>
       <c r="E5">
         <f>C5*D5</f>
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -795,7 +802,7 @@
         <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -808,7 +815,7 @@
         <v>270</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -816,7 +823,7 @@
         <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -834,7 +841,7 @@
         <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8">
         <v>6</v>
@@ -852,7 +859,7 @@
         <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -870,7 +877,7 @@
         <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -888,7 +895,7 @@
         <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11">
         <v>4</v>
@@ -924,7 +931,7 @@
         <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13">
         <v>8</v>
@@ -960,7 +967,7 @@
         <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -978,7 +985,7 @@
         <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -995,7 +1002,7 @@
       <c r="D17" s="1"/>
       <c r="E17">
         <f>SUM(E5:E16)</f>
-        <v>1466</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UPDATED SPREADSHEET WITH CUE AMOUNTS
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="80">
   <si>
     <t>SONG</t>
   </si>
@@ -231,13 +231,46 @@
   </si>
   <si>
     <t>CDC-9393</t>
+  </si>
+  <si>
+    <t>BALLISTIC (POWERHOUSE)</t>
+  </si>
+  <si>
+    <t>DRAGON SPAWN</t>
+  </si>
+  <si>
+    <t>PIRATES BOUNTY</t>
+  </si>
+  <si>
+    <t>SCREAM DREAM</t>
+  </si>
+  <si>
+    <t>PRISMATIC</t>
+  </si>
+  <si>
+    <t>STARGUN</t>
+  </si>
+  <si>
+    <t>DETONATOR 2</t>
+  </si>
+  <si>
+    <t>GREEDY GOBLINS</t>
+  </si>
+  <si>
+    <t>*** HANDS FIREWORKS WEBSITE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 16 PCS 21 CUES</t>
+  </si>
+  <si>
+    <t>50 PCS  39 CUES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,6 +331,13 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -401,7 +441,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -414,6 +454,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="5"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="6"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -706,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:H92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,947 +787,825 @@
       <c r="A2" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="12">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <f>C2*D2</f>
+        <v>20</v>
+      </c>
       <c r="H2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>40</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E9" si="0">C3*D3</f>
+        <v>40</v>
+      </c>
       <c r="H3" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>4</v>
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>29</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>58</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>52</v>
+      <c r="A5" t="s">
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5" s="11">
-        <v>35</v>
+      <c r="D5" s="2">
+        <v>16</v>
       </c>
       <c r="E5">
-        <f>C5*D5</f>
-        <v>70</v>
+        <f t="shared" si="0"/>
+        <v>32</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>52</v>
+      <c r="A6" t="s">
+        <v>55</v>
       </c>
       <c r="B6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>28</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
         <v>56</v>
-      </c>
-      <c r="C6">
-        <v>10</v>
-      </c>
-      <c r="D6" s="4">
-        <v>27</v>
-      </c>
-      <c r="E6">
-        <f t="shared" ref="E6:E16" si="0">C6*D6</f>
-        <v>270</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>52</v>
+      <c r="A7" t="s">
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7" s="5">
-        <v>7.5</v>
+        <v>3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>9</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>52</v>
+      <c r="A8" t="s">
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="C8">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4">
-        <v>43</v>
+        <v>2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>47</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>258</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>52</v>
+      <c r="A9" t="s">
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
-      <c r="D9" s="9">
-        <v>7</v>
+      <c r="D9" s="2">
+        <v>20</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" s="8">
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10">
+        <f>SUM(E2:E9)</f>
+        <v>367</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11">
+      <c r="B14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="4">
-        <v>6</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="7">
-        <v>7</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13">
-        <v>8</v>
-      </c>
-      <c r="D13" s="4">
-        <v>65</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>520</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14">
-        <v>4</v>
-      </c>
-      <c r="D14" s="7">
-        <v>35</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>140</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" s="10">
-        <v>55</v>
+        <v>2</v>
+      </c>
+      <c r="D15" s="11">
+        <v>35</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <f>C15*D15</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" s="9">
+        <v>10</v>
+      </c>
+      <c r="D16" s="4">
+        <v>27</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ref="E16:E26" si="1">C16*D16</f>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="1"/>
-      <c r="E17">
-        <f>SUM(E5:E16)</f>
-        <v>1440</v>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18" s="4">
+        <v>43</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>258</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="9">
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" s="8">
         <v>0</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21">
+        <v>6</v>
+      </c>
+      <c r="D21" s="4">
+        <v>6</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" s="4">
+        <v>30</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23" s="4">
+        <v>65</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24" s="7">
+        <v>35</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25">
         <v>3</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23">
-        <v>32</v>
-      </c>
-      <c r="E23">
-        <f>C23*D23</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24">
-        <v>19</v>
-      </c>
-      <c r="E24">
-        <f t="shared" ref="E24:E37" si="1">C24*D24</f>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <v>33</v>
+      <c r="D25" s="10">
+        <v>55</v>
       </c>
       <c r="E25">
         <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>5</v>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="C26">
-        <v>3</v>
-      </c>
-      <c r="D26">
-        <v>41</v>
+        <v>1</v>
+      </c>
+      <c r="D26" s="9">
+        <v>52</v>
       </c>
       <c r="E26">
         <f t="shared" si="1"/>
-        <v>123</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27">
+        <f>SUM(E15:E26)</f>
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="5">
-        <v>65</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="1"/>
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28">
-        <v>30</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29" s="5">
-        <v>8</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="1"/>
-        <v>16</v>
+      <c r="C29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30">
-        <v>2</v>
-      </c>
-      <c r="D30">
-        <v>34</v>
-      </c>
-      <c r="E30">
-        <f t="shared" si="1"/>
-        <v>68</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D30" s="12"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31" s="2">
-        <v>30</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32">
-        <v>29</v>
-      </c>
-      <c r="E32">
-        <f t="shared" si="1"/>
-        <v>29</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33">
-        <v>2</v>
-      </c>
-      <c r="D33">
-        <v>19</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34">
-        <v>3</v>
-      </c>
-      <c r="D34">
-        <v>47</v>
-      </c>
-      <c r="E34">
-        <f t="shared" si="1"/>
-        <v>141</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" t="s">
-        <v>18</v>
-      </c>
-      <c r="C35">
-        <v>2</v>
-      </c>
-      <c r="D35">
-        <v>29</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="1"/>
-        <v>58</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" t="s">
-        <v>19</v>
-      </c>
-      <c r="C36">
-        <v>3</v>
-      </c>
-      <c r="D36">
-        <v>13</v>
-      </c>
-      <c r="E36">
-        <f t="shared" si="1"/>
-        <v>39</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>5</v>
       </c>
-      <c r="B37" t="s">
-        <v>20</v>
-      </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="D37" s="5">
-        <v>48</v>
-      </c>
-      <c r="E37">
-        <f t="shared" si="1"/>
-        <v>96</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D38" s="1"/>
-      <c r="E38" s="6">
-        <f>SUM(E23:E37)</f>
-        <v>898</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D41" s="1"/>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>32</v>
+      </c>
+      <c r="E41">
+        <f>C41*D41</f>
+        <v>64</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>4</v>
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>19</v>
+      </c>
+      <c r="E42">
+        <f t="shared" ref="E42:E55" si="2">C42*D42</f>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C43">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D43">
-        <v>33.5</v>
+        <v>33</v>
       </c>
       <c r="E43">
-        <f>C43*D43</f>
-        <v>100.5</v>
+        <f t="shared" si="2"/>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C44">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D44">
-        <v>29.95</v>
+        <v>41</v>
       </c>
       <c r="E44">
-        <f t="shared" ref="E44:E73" si="2">C44*D44</f>
-        <v>119.8</v>
+        <f t="shared" si="2"/>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
-      <c r="D45">
-        <v>28.75</v>
+      <c r="D45" s="5">
+        <v>65</v>
       </c>
       <c r="E45">
         <f t="shared" si="2"/>
-        <v>28.75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C46">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D46">
-        <v>3.6</v>
+        <v>30</v>
       </c>
       <c r="E46">
         <f t="shared" si="2"/>
-        <v>57.6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="D47">
-        <v>28.1</v>
+        <v>2</v>
+      </c>
+      <c r="D47" s="5">
+        <v>8</v>
       </c>
       <c r="E47">
         <f t="shared" si="2"/>
-        <v>28.1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C48">
         <v>2</v>
       </c>
       <c r="D48">
-        <v>32.4</v>
+        <v>34</v>
       </c>
       <c r="E48">
         <f t="shared" si="2"/>
-        <v>64.8</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B49" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C49">
-        <v>3</v>
-      </c>
-      <c r="D49">
-        <v>20.100000000000001</v>
+        <v>1</v>
+      </c>
+      <c r="D49" s="2">
+        <v>30</v>
       </c>
       <c r="E49">
         <f t="shared" si="2"/>
-        <v>60.300000000000004</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B50" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D50">
-        <v>34.950000000000003</v>
+        <v>29</v>
       </c>
       <c r="E50">
         <f t="shared" si="2"/>
-        <v>69.900000000000006</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D51">
-        <v>36.950000000000003</v>
+        <v>19</v>
       </c>
       <c r="E51">
         <f t="shared" si="2"/>
-        <v>36.950000000000003</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B52" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D52">
-        <v>12.75</v>
+        <v>47</v>
       </c>
       <c r="E52">
         <f t="shared" si="2"/>
-        <v>25.5</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B53" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C53">
         <v>2</v>
       </c>
       <c r="D53">
-        <v>21.25</v>
+        <v>29</v>
       </c>
       <c r="E53">
         <f t="shared" si="2"/>
-        <v>42.5</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B54" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D54">
-        <v>34.200000000000003</v>
+        <v>13</v>
       </c>
       <c r="E54">
         <f t="shared" si="2"/>
-        <v>34.200000000000003</v>
+        <v>39</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B55" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C55">
-        <v>6</v>
-      </c>
-      <c r="D55">
-        <v>8.9499999999999993</v>
+        <v>2</v>
+      </c>
+      <c r="D55" s="5">
+        <v>48</v>
       </c>
       <c r="E55">
         <f t="shared" si="2"/>
-        <v>53.699999999999996</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>22</v>
-      </c>
-      <c r="B56" t="s">
-        <v>33</v>
-      </c>
       <c r="C56">
-        <v>2</v>
-      </c>
-      <c r="D56" s="4">
-        <v>27.75</v>
-      </c>
-      <c r="E56">
-        <f t="shared" si="2"/>
-        <v>55.5</v>
+        <f>SUM(C41:C55)</f>
+        <v>29</v>
+      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" s="6">
+        <f>SUM(E41:E55)</f>
+        <v>898</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>22</v>
-      </c>
-      <c r="B57" t="s">
-        <v>34</v>
-      </c>
-      <c r="C57">
-        <v>5</v>
-      </c>
-      <c r="D57" s="4">
-        <v>10.5</v>
-      </c>
-      <c r="E57">
-        <f t="shared" si="2"/>
-        <v>52.5</v>
+      <c r="A57" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>22</v>
-      </c>
-      <c r="B58" t="s">
-        <v>35</v>
-      </c>
-      <c r="C58">
-        <v>2</v>
-      </c>
-      <c r="D58">
-        <v>35.950000000000003</v>
-      </c>
-      <c r="E58">
-        <f t="shared" si="2"/>
-        <v>71.900000000000006</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="D58" s="1"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>22</v>
-      </c>
-      <c r="B59" t="s">
-        <v>36</v>
-      </c>
-      <c r="C59">
-        <v>2</v>
-      </c>
-      <c r="D59">
-        <v>29.75</v>
-      </c>
-      <c r="E59">
-        <f t="shared" si="2"/>
-        <v>59.5</v>
-      </c>
+      <c r="D59" s="1"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>22</v>
-      </c>
-      <c r="B60" t="s">
-        <v>37</v>
-      </c>
-      <c r="C60">
-        <v>2</v>
-      </c>
-      <c r="D60">
-        <v>24.75</v>
-      </c>
-      <c r="E60">
-        <f t="shared" si="2"/>
-        <v>49.5</v>
+      <c r="A60" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1694,17 +1613,17 @@
         <v>22</v>
       </c>
       <c r="B61" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C61">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D61">
-        <v>28.95</v>
+        <v>33.5</v>
       </c>
       <c r="E61">
-        <f t="shared" si="2"/>
-        <v>57.9</v>
+        <f>C61*D61</f>
+        <v>100.5</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1712,17 +1631,17 @@
         <v>22</v>
       </c>
       <c r="B62" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D62">
-        <v>19.95</v>
+        <v>29.95</v>
       </c>
       <c r="E62">
-        <f t="shared" si="2"/>
-        <v>19.95</v>
+        <f t="shared" ref="E62:E91" si="3">C62*D62</f>
+        <v>119.8</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1730,17 +1649,17 @@
         <v>22</v>
       </c>
       <c r="B63" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="C63">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D63">
-        <v>26.95</v>
+        <v>28.75</v>
       </c>
       <c r="E63">
-        <f>C63*D63</f>
-        <v>53.9</v>
+        <f t="shared" si="3"/>
+        <v>28.75</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1748,17 +1667,17 @@
         <v>22</v>
       </c>
       <c r="B64" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C64">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D64">
-        <v>23.25</v>
+        <v>3.6</v>
       </c>
       <c r="E64">
-        <f t="shared" si="2"/>
-        <v>46.5</v>
+        <f t="shared" si="3"/>
+        <v>57.6</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -1766,17 +1685,17 @@
         <v>22</v>
       </c>
       <c r="B65" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D65">
-        <v>33.9</v>
+        <v>28.1</v>
       </c>
       <c r="E65">
-        <f t="shared" si="2"/>
-        <v>67.8</v>
+        <f t="shared" si="3"/>
+        <v>28.1</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -1784,17 +1703,17 @@
         <v>22</v>
       </c>
       <c r="B66" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C66">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D66">
-        <v>34.200000000000003</v>
+        <v>32.4</v>
       </c>
       <c r="E66">
-        <f t="shared" si="2"/>
-        <v>102.60000000000001</v>
+        <f t="shared" si="3"/>
+        <v>64.8</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -1802,17 +1721,17 @@
         <v>22</v>
       </c>
       <c r="B67" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D67">
-        <v>50.85</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="E67">
-        <f t="shared" si="2"/>
-        <v>50.85</v>
+        <f t="shared" si="3"/>
+        <v>60.300000000000004</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -1820,17 +1739,17 @@
         <v>22</v>
       </c>
       <c r="B68" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C68">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D68">
-        <v>41.1</v>
+        <v>34.950000000000003</v>
       </c>
       <c r="E68">
-        <f t="shared" si="2"/>
-        <v>164.4</v>
+        <f t="shared" si="3"/>
+        <v>69.900000000000006</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -1838,17 +1757,17 @@
         <v>22</v>
       </c>
       <c r="B69" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D69">
-        <v>41.1</v>
+        <v>36.950000000000003</v>
       </c>
       <c r="E69">
-        <f t="shared" si="2"/>
-        <v>82.2</v>
+        <f t="shared" si="3"/>
+        <v>36.950000000000003</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1856,17 +1775,17 @@
         <v>22</v>
       </c>
       <c r="B70" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="C70">
         <v>2</v>
       </c>
       <c r="D70">
-        <v>22.75</v>
+        <v>12.75</v>
       </c>
       <c r="E70">
-        <f t="shared" si="2"/>
-        <v>45.5</v>
+        <f t="shared" si="3"/>
+        <v>25.5</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -1874,17 +1793,17 @@
         <v>22</v>
       </c>
       <c r="B71" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C71">
         <v>2</v>
       </c>
       <c r="D71">
-        <v>29</v>
+        <v>21.25</v>
       </c>
       <c r="E71">
-        <f t="shared" si="2"/>
-        <v>58</v>
+        <f t="shared" si="3"/>
+        <v>42.5</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1892,17 +1811,17 @@
         <v>22</v>
       </c>
       <c r="B72" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C72">
-        <v>4</v>
-      </c>
-      <c r="D72" s="4">
-        <v>10.5</v>
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>34.200000000000003</v>
       </c>
       <c r="E72">
-        <f t="shared" si="2"/>
-        <v>42</v>
+        <f t="shared" si="3"/>
+        <v>34.200000000000003</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -1910,22 +1829,350 @@
         <v>22</v>
       </c>
       <c r="B73" t="s">
+        <v>32</v>
+      </c>
+      <c r="C73">
+        <v>6</v>
+      </c>
+      <c r="D73">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="3"/>
+        <v>53.699999999999996</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>22</v>
+      </c>
+      <c r="B74" t="s">
+        <v>33</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+      <c r="D74" s="4">
+        <v>27.75</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="3"/>
+        <v>55.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>22</v>
+      </c>
+      <c r="B75" t="s">
+        <v>34</v>
+      </c>
+      <c r="C75">
+        <v>5</v>
+      </c>
+      <c r="D75" s="4">
+        <v>10.5</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="3"/>
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>22</v>
+      </c>
+      <c r="B76" t="s">
+        <v>35</v>
+      </c>
+      <c r="C76">
+        <v>2</v>
+      </c>
+      <c r="D76">
+        <v>35.950000000000003</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="3"/>
+        <v>71.900000000000006</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>22</v>
+      </c>
+      <c r="B77" t="s">
+        <v>36</v>
+      </c>
+      <c r="C77">
+        <v>2</v>
+      </c>
+      <c r="D77">
+        <v>29.75</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="3"/>
+        <v>59.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>22</v>
+      </c>
+      <c r="B78" t="s">
+        <v>37</v>
+      </c>
+      <c r="C78">
+        <v>2</v>
+      </c>
+      <c r="D78">
+        <v>24.75</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="3"/>
+        <v>49.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>22</v>
+      </c>
+      <c r="B79" t="s">
+        <v>38</v>
+      </c>
+      <c r="C79">
+        <v>2</v>
+      </c>
+      <c r="D79">
+        <v>28.95</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="3"/>
+        <v>57.9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>22</v>
+      </c>
+      <c r="B80" t="s">
+        <v>39</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80">
+        <v>19.95</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="3"/>
+        <v>19.95</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>22</v>
+      </c>
+      <c r="B81" t="s">
+        <v>40</v>
+      </c>
+      <c r="C81">
+        <v>2</v>
+      </c>
+      <c r="D81">
+        <v>26.95</v>
+      </c>
+      <c r="E81">
+        <f>C81*D81</f>
+        <v>53.9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>22</v>
+      </c>
+      <c r="B82" t="s">
+        <v>41</v>
+      </c>
+      <c r="C82">
+        <v>2</v>
+      </c>
+      <c r="D82">
+        <v>23.25</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="3"/>
+        <v>46.5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>22</v>
+      </c>
+      <c r="B83" t="s">
+        <v>13</v>
+      </c>
+      <c r="C83">
+        <v>2</v>
+      </c>
+      <c r="D83">
+        <v>33.9</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="3"/>
+        <v>67.8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>22</v>
+      </c>
+      <c r="B84" t="s">
+        <v>42</v>
+      </c>
+      <c r="C84">
+        <v>3</v>
+      </c>
+      <c r="D84">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="3"/>
+        <v>102.60000000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>22</v>
+      </c>
+      <c r="B85" t="s">
+        <v>43</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>50.85</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="3"/>
+        <v>50.85</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>22</v>
+      </c>
+      <c r="B86" t="s">
+        <v>44</v>
+      </c>
+      <c r="C86">
+        <v>4</v>
+      </c>
+      <c r="D86">
+        <v>41.1</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="3"/>
+        <v>164.4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>22</v>
+      </c>
+      <c r="B87" t="s">
+        <v>45</v>
+      </c>
+      <c r="C87">
+        <v>2</v>
+      </c>
+      <c r="D87">
+        <v>41.1</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="3"/>
+        <v>82.2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>22</v>
+      </c>
+      <c r="B88" t="s">
+        <v>46</v>
+      </c>
+      <c r="C88">
+        <v>2</v>
+      </c>
+      <c r="D88">
+        <v>22.75</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="3"/>
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>22</v>
+      </c>
+      <c r="B89" t="s">
+        <v>47</v>
+      </c>
+      <c r="C89">
+        <v>2</v>
+      </c>
+      <c r="D89">
+        <v>29</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>22</v>
+      </c>
+      <c r="B90" t="s">
+        <v>48</v>
+      </c>
+      <c r="C90">
+        <v>4</v>
+      </c>
+      <c r="D90" s="4">
+        <v>10.5</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>22</v>
+      </c>
+      <c r="B91" t="s">
         <v>49</v>
       </c>
-      <c r="C73">
-        <v>2</v>
-      </c>
-      <c r="D73" s="4">
+      <c r="C91">
+        <v>2</v>
+      </c>
+      <c r="D91" s="4">
         <v>4.5</v>
       </c>
-      <c r="E73">
-        <f t="shared" si="2"/>
+      <c r="E91">
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E74" s="6">
-        <f>SUM(E43:E73)</f>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C92">
+        <f>SUM(C61:C91)</f>
+        <v>86</v>
+      </c>
+      <c r="E92" s="6">
+        <f>SUM(E61:E91)</f>
         <v>1812.1000000000004</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated number of Mines in fiddlers;  completed first run on SateliteDiagrams with notes;  starting CueTimes (added file);  updated cueCountPerSong for fiddlers; padded anthemDevil with 10 second buffer.
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="104">
   <si>
     <t>SONG</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>EVIL ENEMY</t>
-  </si>
-  <si>
-    <t>38 PCS 46 CUES</t>
   </si>
   <si>
     <t>61 CUES</t>
@@ -824,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,7 +850,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
@@ -867,7 +864,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -891,7 +888,7 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -915,7 +912,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -939,7 +936,7 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -963,7 +960,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -987,7 +984,7 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -1011,7 +1008,7 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1032,7 +1029,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -1077,7 +1074,7 @@
         <v>3</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>4</v>
@@ -1088,7 +1085,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -1109,7 +1106,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C16">
         <v>10</v>
@@ -1130,7 +1127,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -1151,7 +1148,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -1172,7 +1169,7 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1193,7 +1190,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1214,7 +1211,7 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21">
         <v>6</v>
@@ -1235,7 +1232,7 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -1256,7 +1253,7 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23">
         <v>8</v>
@@ -1277,7 +1274,7 @@
         <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24">
         <v>4</v>
@@ -1298,7 +1295,7 @@
         <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -1319,7 +1316,7 @@
         <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1360,7 +1357,7 @@
         <v>3</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>4</v>
@@ -1371,7 +1368,7 @@
         <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C30">
         <v>7</v>
@@ -1392,7 +1389,7 @@
         <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1413,7 +1410,7 @@
         <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1434,7 +1431,7 @@
         <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -1455,7 +1452,7 @@
         <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C34">
         <v>6</v>
@@ -1476,7 +1473,7 @@
         <v>13</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C35">
         <v>3</v>
@@ -1497,7 +1494,7 @@
         <v>13</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C36">
         <v>13</v>
@@ -1518,7 +1515,7 @@
         <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37">
         <v>3</v>
@@ -1539,7 +1536,7 @@
         <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C38">
         <v>4</v>
@@ -1560,7 +1557,7 @@
         <v>13</v>
       </c>
       <c r="B39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C39">
         <v>4</v>
@@ -1581,7 +1578,7 @@
         <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C40">
         <v>4</v>
@@ -1602,7 +1599,7 @@
         <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C41">
         <v>3</v>
@@ -1623,7 +1620,7 @@
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C42">
         <v>4</v>
@@ -1644,7 +1641,7 @@
         <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C43">
         <v>2</v>
@@ -1665,7 +1662,7 @@
         <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C44">
         <v>4</v>
@@ -1683,7 +1680,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F45">
         <f>SUM(F30:F44)</f>
@@ -1713,7 +1710,7 @@
         <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C47">
         <v>2</v>
@@ -1734,7 +1731,7 @@
         <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C48">
         <v>2</v>
@@ -1755,7 +1752,7 @@
         <v>5</v>
       </c>
       <c r="B49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -1776,7 +1773,7 @@
         <v>5</v>
       </c>
       <c r="B50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C50">
         <v>3</v>
@@ -1797,7 +1794,7 @@
         <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -1818,7 +1815,7 @@
         <v>5</v>
       </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C52">
         <v>2</v>
@@ -1839,7 +1836,7 @@
         <v>5</v>
       </c>
       <c r="B53" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C53">
         <v>2</v>
@@ -1860,7 +1857,7 @@
         <v>5</v>
       </c>
       <c r="B54" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C54">
         <v>2</v>
@@ -1881,7 +1878,7 @@
         <v>5</v>
       </c>
       <c r="B55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -1902,7 +1899,7 @@
         <v>5</v>
       </c>
       <c r="B56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -1923,7 +1920,7 @@
         <v>5</v>
       </c>
       <c r="B57" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C57">
         <v>2</v>
@@ -1944,7 +1941,7 @@
         <v>5</v>
       </c>
       <c r="B58" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C58">
         <v>3</v>
@@ -1965,7 +1962,7 @@
         <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C59">
         <v>2</v>
@@ -1986,7 +1983,7 @@
         <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C60">
         <v>3</v>
@@ -2007,7 +2004,7 @@
         <v>5</v>
       </c>
       <c r="B61" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C61">
         <v>2</v>
@@ -2049,7 +2046,7 @@
         <v>3</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>4</v>
@@ -2060,7 +2057,7 @@
         <v>12</v>
       </c>
       <c r="B64" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C64">
         <v>4</v>
@@ -2081,7 +2078,7 @@
         <v>12</v>
       </c>
       <c r="B65" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C65">
         <v>2</v>
@@ -2108,7 +2105,7 @@
         <v>2</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E66" s="1">
         <v>0</v>
@@ -2123,7 +2120,7 @@
         <v>12</v>
       </c>
       <c r="B67" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C67">
         <v>2</v>
@@ -2144,13 +2141,13 @@
         <v>12</v>
       </c>
       <c r="B68" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C68">
         <v>3</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E68" s="1">
         <v>0</v>
@@ -2165,10 +2162,10 @@
         <v>12</v>
       </c>
       <c r="B69" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C69">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D69">
         <v>10.5</v>
@@ -2178,7 +2175,7 @@
       </c>
       <c r="F69">
         <f t="shared" si="4"/>
-        <v>37.799999999999997</v>
+        <v>56.699999999999996</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2186,7 +2183,7 @@
         <v>12</v>
       </c>
       <c r="B70" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C70">
         <v>2</v>
@@ -2207,7 +2204,7 @@
         <v>12</v>
       </c>
       <c r="B71" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C71">
         <v>4</v>
@@ -2228,10 +2225,10 @@
         <v>12</v>
       </c>
       <c r="B72" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C72">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D72">
         <v>9.25</v>
@@ -2241,7 +2238,7 @@
       </c>
       <c r="F72">
         <f t="shared" si="4"/>
-        <v>83.25</v>
+        <v>138.75</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2249,7 +2246,7 @@
         <v>12</v>
       </c>
       <c r="B73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C73">
         <v>4</v>
@@ -2266,13 +2263,14 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C74" t="s">
-        <v>25</v>
+      <c r="C74">
+        <f>SUM(C64:C73)</f>
+        <v>47</v>
       </c>
       <c r="D74" s="1"/>
       <c r="F74">
         <f>SUM(F64:F73)</f>
-        <v>497.35</v>
+        <v>571.75</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2295,7 +2293,7 @@
         <v>3</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>4</v>
@@ -2306,7 +2304,7 @@
         <v>7</v>
       </c>
       <c r="B78" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C78">
         <v>3</v>
@@ -2318,7 +2316,7 @@
         <v>33.5</v>
       </c>
       <c r="F78">
-        <f>C78*D78</f>
+        <f t="shared" ref="F78:F107" si="5">C78*D78</f>
         <v>100.5</v>
       </c>
     </row>
@@ -2327,7 +2325,7 @@
         <v>7</v>
       </c>
       <c r="B79" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C79">
         <v>4</v>
@@ -2339,7 +2337,7 @@
         <v>29.95</v>
       </c>
       <c r="F79">
-        <f>C79*D79</f>
+        <f t="shared" si="5"/>
         <v>119.8</v>
       </c>
     </row>
@@ -2348,7 +2346,7 @@
         <v>7</v>
       </c>
       <c r="B80" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -2360,7 +2358,7 @@
         <v>28.75</v>
       </c>
       <c r="F80">
-        <f>C80*D80</f>
+        <f t="shared" si="5"/>
         <v>28.75</v>
       </c>
     </row>
@@ -2369,7 +2367,7 @@
         <v>7</v>
       </c>
       <c r="B81" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C81">
         <v>16</v>
@@ -2381,7 +2379,7 @@
         <v>2.85</v>
       </c>
       <c r="F81">
-        <f>C81*D81</f>
+        <f t="shared" si="5"/>
         <v>76</v>
       </c>
     </row>
@@ -2390,7 +2388,7 @@
         <v>7</v>
       </c>
       <c r="B82" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -2402,7 +2400,7 @@
         <v>28.1</v>
       </c>
       <c r="F82">
-        <f>C82*D82</f>
+        <f t="shared" si="5"/>
         <v>28.1</v>
       </c>
     </row>
@@ -2411,7 +2409,7 @@
         <v>7</v>
       </c>
       <c r="B83" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C83">
         <v>2</v>
@@ -2423,7 +2421,7 @@
         <v>32.4</v>
       </c>
       <c r="F83">
-        <f>C83*D83</f>
+        <f t="shared" si="5"/>
         <v>64.8</v>
       </c>
     </row>
@@ -2432,7 +2430,7 @@
         <v>7</v>
       </c>
       <c r="B84" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C84">
         <v>3</v>
@@ -2444,7 +2442,7 @@
         <v>20.100000000000001</v>
       </c>
       <c r="F84">
-        <f>C84*D84</f>
+        <f t="shared" si="5"/>
         <v>60.300000000000004</v>
       </c>
     </row>
@@ -2453,7 +2451,7 @@
         <v>7</v>
       </c>
       <c r="B85" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C85">
         <v>2</v>
@@ -2465,7 +2463,7 @@
         <v>34.950000000000003</v>
       </c>
       <c r="F85">
-        <f>C85*D85</f>
+        <f t="shared" si="5"/>
         <v>69.900000000000006</v>
       </c>
     </row>
@@ -2474,7 +2472,7 @@
         <v>7</v>
       </c>
       <c r="B86" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -2486,7 +2484,7 @@
         <v>36.950000000000003</v>
       </c>
       <c r="F86">
-        <f>C86*D86</f>
+        <f t="shared" si="5"/>
         <v>36.950000000000003</v>
       </c>
     </row>
@@ -2495,7 +2493,7 @@
         <v>7</v>
       </c>
       <c r="B87" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C87">
         <v>2</v>
@@ -2507,7 +2505,7 @@
         <v>12.75</v>
       </c>
       <c r="F87">
-        <f>C87*D87</f>
+        <f t="shared" si="5"/>
         <v>25.5</v>
       </c>
     </row>
@@ -2516,7 +2514,7 @@
         <v>7</v>
       </c>
       <c r="B88" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C88">
         <v>2</v>
@@ -2528,7 +2526,7 @@
         <v>21.25</v>
       </c>
       <c r="F88">
-        <f>C88*D88</f>
+        <f t="shared" si="5"/>
         <v>42.5</v>
       </c>
     </row>
@@ -2537,7 +2535,7 @@
         <v>7</v>
       </c>
       <c r="B89" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C89">
         <v>1</v>
@@ -2549,7 +2547,7 @@
         <v>34.200000000000003</v>
       </c>
       <c r="F89">
-        <f>C89*D89</f>
+        <f t="shared" si="5"/>
         <v>34.200000000000003</v>
       </c>
     </row>
@@ -2558,7 +2556,7 @@
         <v>7</v>
       </c>
       <c r="B90" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C90">
         <v>6</v>
@@ -2570,7 +2568,7 @@
         <v>8.9499999999999993</v>
       </c>
       <c r="F90">
-        <f>C90*D90</f>
+        <f t="shared" si="5"/>
         <v>53.699999999999996</v>
       </c>
     </row>
@@ -2579,7 +2577,7 @@
         <v>7</v>
       </c>
       <c r="B91" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C91">
         <v>2</v>
@@ -2591,7 +2589,7 @@
         <v>27.75</v>
       </c>
       <c r="F91">
-        <f>C91*D91</f>
+        <f t="shared" si="5"/>
         <v>55.5</v>
       </c>
     </row>
@@ -2600,7 +2598,7 @@
         <v>7</v>
       </c>
       <c r="B92" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C92">
         <v>5</v>
@@ -2612,7 +2610,7 @@
         <v>10.5</v>
       </c>
       <c r="F92">
-        <f>C92*D92</f>
+        <f t="shared" si="5"/>
         <v>52.5</v>
       </c>
     </row>
@@ -2621,7 +2619,7 @@
         <v>7</v>
       </c>
       <c r="B93" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C93">
         <v>2</v>
@@ -2630,7 +2628,7 @@
         <v>35.950000000000003</v>
       </c>
       <c r="F93">
-        <f>C93*D93</f>
+        <f t="shared" si="5"/>
         <v>71.900000000000006</v>
       </c>
     </row>
@@ -2639,7 +2637,7 @@
         <v>7</v>
       </c>
       <c r="B94" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C94">
         <v>2</v>
@@ -2648,7 +2646,7 @@
         <v>29.75</v>
       </c>
       <c r="F94">
-        <f>C94*D94</f>
+        <f t="shared" si="5"/>
         <v>59.5</v>
       </c>
     </row>
@@ -2657,7 +2655,7 @@
         <v>7</v>
       </c>
       <c r="B95" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C95">
         <v>2</v>
@@ -2666,7 +2664,7 @@
         <v>24.75</v>
       </c>
       <c r="F95">
-        <f>C95*D95</f>
+        <f t="shared" si="5"/>
         <v>49.5</v>
       </c>
     </row>
@@ -2684,7 +2682,7 @@
         <v>28.95</v>
       </c>
       <c r="F96">
-        <f>C96*D96</f>
+        <f t="shared" si="5"/>
         <v>57.9</v>
       </c>
     </row>
@@ -2693,7 +2691,7 @@
         <v>7</v>
       </c>
       <c r="B97" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C97">
         <v>1</v>
@@ -2702,7 +2700,7 @@
         <v>19.95</v>
       </c>
       <c r="F97">
-        <f>C97*D97</f>
+        <f t="shared" si="5"/>
         <v>19.95</v>
       </c>
     </row>
@@ -2711,7 +2709,7 @@
         <v>7</v>
       </c>
       <c r="B98" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C98">
         <v>2</v>
@@ -2720,7 +2718,7 @@
         <v>26.95</v>
       </c>
       <c r="F98">
-        <f>C98*D98</f>
+        <f t="shared" si="5"/>
         <v>53.9</v>
       </c>
     </row>
@@ -2729,7 +2727,7 @@
         <v>7</v>
       </c>
       <c r="B99" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C99">
         <v>2</v>
@@ -2738,7 +2736,7 @@
         <v>23.25</v>
       </c>
       <c r="F99">
-        <f>C99*D99</f>
+        <f t="shared" si="5"/>
         <v>46.5</v>
       </c>
     </row>
@@ -2747,7 +2745,7 @@
         <v>7</v>
       </c>
       <c r="B100" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C100">
         <v>2</v>
@@ -2756,7 +2754,7 @@
         <v>33.9</v>
       </c>
       <c r="F100">
-        <f>C100*D100</f>
+        <f t="shared" si="5"/>
         <v>67.8</v>
       </c>
     </row>
@@ -2765,7 +2763,7 @@
         <v>7</v>
       </c>
       <c r="B101" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C101">
         <v>3</v>
@@ -2774,7 +2772,7 @@
         <v>34.200000000000003</v>
       </c>
       <c r="F101">
-        <f>C101*D101</f>
+        <f t="shared" si="5"/>
         <v>102.60000000000001</v>
       </c>
     </row>
@@ -2792,7 +2790,7 @@
         <v>50.85</v>
       </c>
       <c r="F102">
-        <f>C102*D102</f>
+        <f t="shared" si="5"/>
         <v>50.85</v>
       </c>
     </row>
@@ -2810,7 +2808,7 @@
         <v>41.1</v>
       </c>
       <c r="F103">
-        <f>C103*D103</f>
+        <f t="shared" si="5"/>
         <v>164.4</v>
       </c>
     </row>
@@ -2828,7 +2826,7 @@
         <v>41.1</v>
       </c>
       <c r="F104">
-        <f>C104*D104</f>
+        <f t="shared" si="5"/>
         <v>82.2</v>
       </c>
     </row>
@@ -2837,7 +2835,7 @@
         <v>7</v>
       </c>
       <c r="B105" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C105">
         <v>2</v>
@@ -2849,7 +2847,7 @@
         <v>24.75</v>
       </c>
       <c r="F105">
-        <f>C105*D105</f>
+        <f t="shared" si="5"/>
         <v>49.5</v>
       </c>
     </row>
@@ -2858,7 +2856,7 @@
         <v>7</v>
       </c>
       <c r="B106" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C106">
         <v>2</v>
@@ -2870,7 +2868,7 @@
         <v>29</v>
       </c>
       <c r="F106">
-        <f>C106*D106</f>
+        <f t="shared" si="5"/>
         <v>58</v>
       </c>
     </row>
@@ -2879,7 +2877,7 @@
         <v>7</v>
       </c>
       <c r="B107" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C107">
         <v>4</v>
@@ -2891,7 +2889,7 @@
         <v>8.4</v>
       </c>
       <c r="F107">
-        <f>C107*D107</f>
+        <f t="shared" si="5"/>
         <v>56</v>
       </c>
     </row>
@@ -2900,7 +2898,7 @@
         <v>7</v>
       </c>
       <c r="B108" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C108">
         <v>2</v>

</xml_diff>

<commit_message>
adjust a few queues that were wrong.  remove emperors tattoo; fix sat diagrams
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -821,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47:C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,6 +1055,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <f>SUM(C2:C9)</f>
+        <v>16</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1343,6 +1347,12 @@
         <v>1229.05</v>
       </c>
     </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <f>SUM(C15:C26)</f>
+        <v>50</v>
+      </c>
+    </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
book one with updated fireworks and quantities
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="101">
   <si>
     <t>SONG</t>
   </si>
@@ -92,18 +92,9 @@
     <t>*** HANDS FIREWORKS WEBSITE</t>
   </si>
   <si>
-    <t xml:space="preserve"> 16 PCS 21 CUES</t>
-  </si>
-  <si>
-    <t>50 PCS  39 CUES</t>
-  </si>
-  <si>
     <t>EVIL ENEMY</t>
   </si>
   <si>
-    <t>61 CUES</t>
-  </si>
-  <si>
     <t>DISCOUNTED PRICE</t>
   </si>
   <si>
@@ -125,9 +116,6 @@
     <t>OVER THE RAINBOW (BEM)</t>
   </si>
   <si>
-    <t>EMPEROR'S TATTOO (MYS)</t>
-  </si>
-  <si>
     <t>MELTDOWN (VUL)</t>
   </si>
   <si>
@@ -194,9 +182,6 @@
     <t>THE PROUD (TNF)</t>
   </si>
   <si>
-    <t>MULTICOLOUR PEONIES (VUL)</t>
-  </si>
-  <si>
     <t>BALLISTIC (PH)</t>
   </si>
   <si>
@@ -293,9 +278,6 @@
     <t>PIRATES BOUNTY (VUL)</t>
   </si>
   <si>
-    <t>DRAGON SPAWN (HANDS)</t>
-  </si>
-  <si>
     <t>SUB ZERO (COMP)</t>
   </si>
   <si>
@@ -320,9 +302,6 @@
     <t>SHELL SHOCKED (PH)</t>
   </si>
   <si>
-    <t>GOLDEN EYE (MYS)</t>
-  </si>
-  <si>
     <t>DOOMS DAY (COMP)</t>
   </si>
   <si>
@@ -336,6 +315,18 @@
   </si>
   <si>
     <t>VOLATILE (COMP)</t>
+  </si>
+  <si>
+    <t>colorful dhalia</t>
+  </si>
+  <si>
+    <t>deleted</t>
+  </si>
+  <si>
+    <t>91 shot kaleidoscopes</t>
+  </si>
+  <si>
+    <t>sub zero</t>
   </si>
 </sst>
 </file>
@@ -821,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47:C62"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="F109" sqref="F67:I109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,7 +841,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
@@ -864,10 +855,10 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D2" s="12">
         <v>10</v>
@@ -877,7 +868,7 @@
       </c>
       <c r="F2">
         <f>C2*E2</f>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I2" t="s">
         <v>6</v>
@@ -888,7 +879,7 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -912,7 +903,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -936,7 +927,7 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -960,7 +951,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -984,7 +975,7 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -1008,7 +999,7 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1029,7 +1020,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -1046,18 +1037,15 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
       <c r="F10">
         <f>SUM(F2:F9)</f>
-        <v>358.5</v>
+        <v>370.5</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11">
         <f>SUM(C2:C9)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -1078,7 +1066,7 @@
         <v>3</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>4</v>
@@ -1089,7 +1077,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -1110,7 +1098,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C16">
         <v>10</v>
@@ -1131,7 +1119,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -1152,7 +1140,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -1173,10 +1161,10 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D19" s="9">
         <v>6.75</v>
@@ -1186,7 +1174,7 @@
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>8.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1194,20 +1182,20 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D20">
-        <v>29.95</v>
+        <v>27</v>
       </c>
       <c r="E20">
-        <v>29.95</v>
+        <v>18</v>
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>59.9</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1215,7 +1203,7 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C21">
         <v>6</v>
@@ -1236,7 +1224,7 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -1257,7 +1245,7 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C23">
         <v>8</v>
@@ -1278,7 +1266,7 @@
         <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C24">
         <v>4</v>
@@ -1299,7 +1287,7 @@
         <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -1320,7 +1308,7 @@
         <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1337,20 +1325,17 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>23</v>
-      </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27">
         <f>SUM(F15:F26)</f>
-        <v>1229.05</v>
+        <v>1269.05</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C28">
         <f>SUM(C15:C26)</f>
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1367,7 +1352,7 @@
         <v>3</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>4</v>
@@ -1378,7 +1363,7 @@
         <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C30">
         <v>7</v>
@@ -1399,7 +1384,7 @@
         <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1420,7 +1405,7 @@
         <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1441,7 +1426,7 @@
         <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -1462,7 +1447,7 @@
         <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C34">
         <v>6</v>
@@ -1483,7 +1468,7 @@
         <v>13</v>
       </c>
       <c r="B35" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C35">
         <v>3</v>
@@ -1504,7 +1489,7 @@
         <v>13</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C36">
         <v>13</v>
@@ -1525,7 +1510,7 @@
         <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C37">
         <v>3</v>
@@ -1546,7 +1531,7 @@
         <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C38">
         <v>4</v>
@@ -1567,7 +1552,7 @@
         <v>13</v>
       </c>
       <c r="B39" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C39">
         <v>4</v>
@@ -1588,7 +1573,7 @@
         <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C40">
         <v>4</v>
@@ -1609,7 +1594,7 @@
         <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C41">
         <v>3</v>
@@ -1630,7 +1615,7 @@
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C42">
         <v>4</v>
@@ -1651,7 +1636,7 @@
         <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C43">
         <v>2</v>
@@ -1672,7 +1657,7 @@
         <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C44">
         <v>4</v>
@@ -1689,8 +1674,9 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>25</v>
+      <c r="C45">
+        <f>SUM(C30:C44)</f>
+        <v>61</v>
       </c>
       <c r="F45">
         <f>SUM(F30:F44)</f>
@@ -1720,7 +1706,7 @@
         <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C47">
         <v>2</v>
@@ -1741,7 +1727,7 @@
         <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C48">
         <v>2</v>
@@ -1762,7 +1748,7 @@
         <v>5</v>
       </c>
       <c r="B49" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -1783,7 +1769,7 @@
         <v>5</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C50">
         <v>3</v>
@@ -1804,7 +1790,7 @@
         <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -1825,7 +1811,7 @@
         <v>5</v>
       </c>
       <c r="B52" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C52">
         <v>2</v>
@@ -1846,7 +1832,7 @@
         <v>5</v>
       </c>
       <c r="B53" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C53">
         <v>2</v>
@@ -1867,7 +1853,7 @@
         <v>5</v>
       </c>
       <c r="B54" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C54">
         <v>2</v>
@@ -1888,7 +1874,7 @@
         <v>5</v>
       </c>
       <c r="B55" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -1909,7 +1895,7 @@
         <v>5</v>
       </c>
       <c r="B56" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -1930,7 +1916,7 @@
         <v>5</v>
       </c>
       <c r="B57" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C57">
         <v>2</v>
@@ -1951,7 +1937,7 @@
         <v>5</v>
       </c>
       <c r="B58" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C58">
         <v>3</v>
@@ -1972,7 +1958,7 @@
         <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C59">
         <v>2</v>
@@ -1993,7 +1979,7 @@
         <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C60">
         <v>3</v>
@@ -2014,7 +2000,7 @@
         <v>5</v>
       </c>
       <c r="B61" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C61">
         <v>2</v>
@@ -2056,7 +2042,7 @@
         <v>3</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>4</v>
@@ -2067,7 +2053,7 @@
         <v>12</v>
       </c>
       <c r="B64" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C64">
         <v>4</v>
@@ -2088,7 +2074,7 @@
         <v>12</v>
       </c>
       <c r="B65" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C65">
         <v>2</v>
@@ -2109,13 +2095,13 @@
         <v>12</v>
       </c>
       <c r="B66" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C66">
         <v>2</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E66" s="1">
         <v>0</v>
@@ -2130,7 +2116,7 @@
         <v>12</v>
       </c>
       <c r="B67" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C67">
         <v>2</v>
@@ -2151,13 +2137,13 @@
         <v>12</v>
       </c>
       <c r="B68" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C68">
         <v>3</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E68" s="1">
         <v>0</v>
@@ -2172,7 +2158,7 @@
         <v>12</v>
       </c>
       <c r="B69" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C69">
         <v>9</v>
@@ -2193,7 +2179,7 @@
         <v>12</v>
       </c>
       <c r="B70" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C70">
         <v>2</v>
@@ -2214,7 +2200,7 @@
         <v>12</v>
       </c>
       <c r="B71" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C71">
         <v>4</v>
@@ -2235,7 +2221,7 @@
         <v>12</v>
       </c>
       <c r="B72" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C72">
         <v>15</v>
@@ -2256,7 +2242,7 @@
         <v>12</v>
       </c>
       <c r="B73" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C73">
         <v>4</v>
@@ -2303,7 +2289,7 @@
         <v>3</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>4</v>
@@ -2314,7 +2300,7 @@
         <v>7</v>
       </c>
       <c r="B78" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C78">
         <v>3</v>
@@ -2335,7 +2321,7 @@
         <v>7</v>
       </c>
       <c r="B79" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C79">
         <v>4</v>
@@ -2356,7 +2342,7 @@
         <v>7</v>
       </c>
       <c r="B80" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -2377,20 +2363,20 @@
         <v>7</v>
       </c>
       <c r="B81" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C81">
         <v>16</v>
       </c>
       <c r="D81" s="4">
-        <v>4.75</v>
+        <v>7</v>
       </c>
       <c r="E81" s="4">
-        <v>2.85</v>
+        <v>5</v>
       </c>
       <c r="F81">
         <f t="shared" si="5"/>
-        <v>76</v>
+        <v>112</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2398,7 +2384,7 @@
         <v>7</v>
       </c>
       <c r="B82" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -2419,7 +2405,7 @@
         <v>7</v>
       </c>
       <c r="B83" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C83">
         <v>2</v>
@@ -2440,7 +2426,7 @@
         <v>7</v>
       </c>
       <c r="B84" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C84">
         <v>3</v>
@@ -2461,7 +2447,7 @@
         <v>7</v>
       </c>
       <c r="B85" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C85">
         <v>2</v>
@@ -2482,7 +2468,7 @@
         <v>7</v>
       </c>
       <c r="B86" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -2503,7 +2489,7 @@
         <v>7</v>
       </c>
       <c r="B87" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C87">
         <v>2</v>
@@ -2524,7 +2510,7 @@
         <v>7</v>
       </c>
       <c r="B88" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C88">
         <v>2</v>
@@ -2545,7 +2531,7 @@
         <v>7</v>
       </c>
       <c r="B89" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C89">
         <v>1</v>
@@ -2566,7 +2552,7 @@
         <v>7</v>
       </c>
       <c r="B90" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C90">
         <v>6</v>
@@ -2587,7 +2573,7 @@
         <v>7</v>
       </c>
       <c r="B91" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C91">
         <v>2</v>
@@ -2608,7 +2594,7 @@
         <v>7</v>
       </c>
       <c r="B92" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C92">
         <v>5</v>
@@ -2629,7 +2615,7 @@
         <v>7</v>
       </c>
       <c r="B93" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C93">
         <v>2</v>
@@ -2647,7 +2633,7 @@
         <v>7</v>
       </c>
       <c r="B94" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C94">
         <v>2</v>
@@ -2665,7 +2651,7 @@
         <v>7</v>
       </c>
       <c r="B95" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C95">
         <v>2</v>
@@ -2701,7 +2687,7 @@
         <v>7</v>
       </c>
       <c r="B97" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C97">
         <v>1</v>
@@ -2719,7 +2705,7 @@
         <v>7</v>
       </c>
       <c r="B98" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C98">
         <v>2</v>
@@ -2737,7 +2723,7 @@
         <v>7</v>
       </c>
       <c r="B99" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C99">
         <v>2</v>
@@ -2755,7 +2741,7 @@
         <v>7</v>
       </c>
       <c r="B100" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C100">
         <v>2</v>
@@ -2773,7 +2759,7 @@
         <v>7</v>
       </c>
       <c r="B101" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C101">
         <v>3</v>
@@ -2845,7 +2831,7 @@
         <v>7</v>
       </c>
       <c r="B105" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C105">
         <v>2</v>
@@ -2866,7 +2852,7 @@
         <v>7</v>
       </c>
       <c r="B106" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C106">
         <v>2</v>
@@ -2887,7 +2873,7 @@
         <v>7</v>
       </c>
       <c r="B107" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C107">
         <v>4</v>
@@ -2908,7 +2894,7 @@
         <v>7</v>
       </c>
       <c r="B108" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C108">
         <v>2</v>
@@ -2927,11 +2913,12 @@
       </c>
       <c r="F109" s="6">
         <f>SUM(F78:F108)</f>
-        <v>1839.5000000000002</v>
+        <v>1875.5000000000002</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>